<commit_message>
Validation steps to look at before/after Step 1&2 clean
</commit_message>
<xml_diff>
--- a/ExtraDetails/ValidateTotals.xlsx
+++ b/ExtraDetails/ValidateTotals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teriko.moriyasu\Documents\GitHub\TerikoTableau\ExtraDetails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC9FA6E-2D97-44F8-A527-E0238E710C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36361986-5E85-40FC-939F-E1E337BA353E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-86400" yWindow="1080" windowWidth="28800" windowHeight="15495" xr2:uid="{41ADC8B9-EB8D-4657-9C4F-3D3145DEA060}"/>
+    <workbookView xWindow="-86520" yWindow="3975" windowWidth="29040" windowHeight="15840" xr2:uid="{41ADC8B9-EB8D-4657-9C4F-3D3145DEA060}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>Product Detail</t>
   </si>
@@ -82,7 +82,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +105,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,14 +142,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -139,10 +175,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
@@ -456,37 +495,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D33402D-BFF9-4AC9-8E8B-0755F2C3E7F9}">
-  <dimension ref="A2:K7"/>
+  <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
+      <c r="G2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -498,14 +546,14 @@
       <c r="C3" s="5">
         <v>46948785</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>9</v>
+      <c r="G3" s="6">
+        <v>44146</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>52894890</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -519,13 +567,13 @@
         <v>4108000</v>
       </c>
       <c r="G4" s="6">
-        <v>44146</v>
+        <v>44169</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I4" s="8">
-        <v>52894890</v>
+        <v>51688087</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -544,14 +592,19 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="6">
-        <v>44169</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="I5" s="8">
-        <v>51688087</v>
+        <f>I3-I4</f>
+        <v>1206803</v>
+      </c>
+      <c r="J5" s="7">
+        <f>100%+I5/I3-1</f>
+        <v>2.2815115032851052E-2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -570,20 +623,6 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="H6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="8">
-        <f>I4-I5</f>
-        <v>1206803</v>
-      </c>
-      <c r="J6" s="7">
-        <f>100%+I6/I4-1</f>
-        <v>2.2815115032851052E-2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -598,6 +637,165 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="6">
+        <v>44173</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8">
+        <v>54207062</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>47632684</v>
+      </c>
+      <c r="D17" s="2">
+        <f>C17-C3</f>
+        <v>683899</v>
+      </c>
+      <c r="G17" s="6">
+        <v>44173</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="8">
+        <v>53006603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4212233</v>
+      </c>
+      <c r="D18" s="2">
+        <f>C18-C4</f>
+        <v>104233</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="8">
+        <f>I16-I17</f>
+        <v>1200459</v>
+      </c>
+      <c r="J18" s="7">
+        <f>100%+I18/I16-1</f>
+        <v>2.2145804544802639E-2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>47632684</v>
+      </c>
+      <c r="D19" s="2">
+        <f>C17-C19</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4212233</v>
+      </c>
+      <c r="D20" s="2">
+        <f>C18-C20</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>14651842</v>
+      </c>
+      <c r="D21" s="2">
+        <f>C21-C7</f>
+        <v>205326</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="C24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Parent ID and Member Status to Step 2 PLUS several mfg mappings
</commit_message>
<xml_diff>
--- a/ExtraDetails/ValidateTotals.xlsx
+++ b/ExtraDetails/ValidateTotals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teriko.moriyasu\Documents\GitHub\TerikoTableau\ExtraDetails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36361986-5E85-40FC-939F-E1E337BA353E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1817D6-211F-4DDB-BF4A-1867F659B49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-86520" yWindow="3975" windowWidth="29040" windowHeight="15840" xr2:uid="{41ADC8B9-EB8D-4657-9C4F-3D3145DEA060}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
   <si>
     <t>Product Detail</t>
   </si>
@@ -69,6 +69,33 @@
   </si>
   <si>
     <t>&lt;-- % lost NVD, some loss was expected</t>
+  </si>
+  <si>
+    <t>COMPARE BEFORE &amp; AFTER RUNNING CLEAN STEPS</t>
+  </si>
+  <si>
+    <t>added manufacturers</t>
+  </si>
+  <si>
+    <t>changed QTR and 1H format</t>
+  </si>
+  <si>
+    <t>tried to add Parent ID and Member Status (but it didn't flow through)</t>
+  </si>
+  <si>
+    <t>What prep things changed</t>
+  </si>
+  <si>
+    <t>reason for smaller PD + NVD count is because I mapped more to the New field, it compressed the number of records</t>
+  </si>
+  <si>
+    <t>added manufacturers mapping</t>
+  </si>
+  <si>
+    <t>pulled in new data from Rosa :)</t>
+  </si>
+  <si>
+    <t>bigger PD+NVD count is because pulled in new data</t>
   </si>
 </sst>
 </file>
@@ -165,7 +192,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -177,6 +204,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -495,9 +523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D33402D-BFF9-4AC9-8E8B-0755F2C3E7F9}">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -509,113 +539,88 @@
     <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="63.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="9" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>44146</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>46948785</v>
-      </c>
-      <c r="G3" s="6">
-        <v>44146</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>52894890</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44146</v>
       </c>
       <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>46948785</v>
+      </c>
+      <c r="G4" s="6">
+        <v>44146</v>
+      </c>
+      <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="I4" s="8">
+        <v>52894890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>44146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
         <v>4108000</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G5" s="6">
         <v>44169</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I5" s="8">
         <v>51688087</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>44169</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>46948785</v>
-      </c>
-      <c r="D5" s="2">
-        <f>C3-C5</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="8">
-        <f>I3-I4</f>
-        <v>1206803</v>
-      </c>
-      <c r="J5" s="7">
-        <f>100%+I5/I3-1</f>
-        <v>2.2815115032851052E-2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44169</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>4108000</v>
+        <v>46948785</v>
       </c>
       <c r="D6" s="2">
         <f>C4-C6</f>
@@ -623,179 +628,366 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="8">
+        <f>I4-I5</f>
+        <v>1206803</v>
+      </c>
+      <c r="J6" s="7">
+        <f>100%+I6/I4-1</f>
+        <v>2.2815115032851052E-2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44169</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>14446516</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>4108000</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C5-C7</f>
+        <v>0</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>44169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14446516</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="6">
+      <c r="L10" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>44173</v>
       </c>
-      <c r="H16" t="s">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>47632684</v>
+      </c>
+      <c r="D11" s="2">
+        <f>C11-C4</f>
+        <v>683899</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="6">
+        <v>44173</v>
+      </c>
+      <c r="H11" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I11" s="8">
         <v>54207062</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="L11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>44173</v>
       </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>4212233</v>
+      </c>
+      <c r="D12" s="2">
+        <f>C12-C5</f>
+        <v>104233</v>
+      </c>
+      <c r="G12" s="6">
+        <v>44173</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="8">
+        <v>53006603</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
         <v>47632684</v>
       </c>
-      <c r="D17" s="2">
-        <f>C17-C3</f>
-        <v>683899</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="D13" s="2">
+        <f>C11-C13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="8">
+        <f>I11-I12</f>
+        <v>1200459</v>
+      </c>
+      <c r="J13" s="7">
+        <f>100%+I13/I11-1</f>
+        <v>2.2145804544802639E-2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>44173</v>
       </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="8">
-        <v>53006603</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4212233</v>
+      </c>
+      <c r="D14" s="2">
+        <f>C12-C14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>44173</v>
       </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="5">
-        <v>4212233</v>
-      </c>
-      <c r="D18" s="2">
-        <f>C18-C4</f>
-        <v>104233</v>
-      </c>
-      <c r="H18" s="4" t="s">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14651842</v>
+      </c>
+      <c r="D15" s="2">
+        <f>C15-C8</f>
+        <v>205326</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="L15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="8">
-        <f>I16-I17</f>
-        <v>1200459</v>
-      </c>
-      <c r="J18" s="7">
-        <f>100%+I18/I16-1</f>
-        <v>2.2145804544802639E-2</v>
-      </c>
-      <c r="K18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>44173</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
         <v>47632684</v>
       </c>
       <c r="D19" s="2">
-        <f>C17-C19</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <f>C19-C11</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="6">
+        <v>44176</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8">
+        <v>54207062</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>44173</v>
       </c>
       <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4212233</v>
+      </c>
+      <c r="D20" s="2">
+        <f>C20-C12</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>44176</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="8">
+        <v>53006603</v>
+      </c>
+      <c r="L20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>44176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>47632684</v>
+      </c>
+      <c r="D21" s="2">
+        <f>C19-C21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="8">
+        <f>I19-I20</f>
+        <v>1200459</v>
+      </c>
+      <c r="J21" s="7">
+        <f>100%+I21/I19-1</f>
+        <v>2.2145804544802639E-2</v>
+      </c>
+      <c r="K21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>44176</v>
+      </c>
+      <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C22" s="1">
         <v>4212233</v>
       </c>
-      <c r="D20" s="2">
-        <f>C18-C20</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>44173</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D22" s="2">
+        <f>C20-C22</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>44176</v>
+      </c>
+      <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="1">
-        <v>14651842</v>
-      </c>
-      <c r="D21" s="2">
-        <f>C21-C7</f>
-        <v>205326</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="C24" s="1"/>
+      <c r="C23" s="1">
+        <v>14651765</v>
+      </c>
+      <c r="D23" s="2">
+        <f>C23-C15</f>
+        <v>-77</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="2"/>
+      <c r="G24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mfg and sector csv updates and new mfg analysis
Manufacturer csv added some mfgs and modified mistakes
Sector csv modified
new versions of Mfg analysis clean
</commit_message>
<xml_diff>
--- a/ExtraDetails/ValidateTotals.xlsx
+++ b/ExtraDetails/ValidateTotals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teriko.moriyasu\Documents\GitHub\TerikoTableau\ExtraDetails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE5D4DD-C702-40B5-A321-5736316BFF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1E7C37-81E2-4E17-9E59-243FEE5837F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{41ADC8B9-EB8D-4657-9C4F-3D3145DEA060}"/>
+    <workbookView xWindow="-86520" yWindow="3975" windowWidth="29040" windowHeight="15840" xr2:uid="{41ADC8B9-EB8D-4657-9C4F-3D3145DEA060}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D33402D-BFF9-4AC9-8E8B-0755F2C3E7F9}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1227,10 +1229,12 @@
       <c r="B36" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1">
+        <v>48107243</v>
+      </c>
       <c r="D36" s="2">
         <f>C36-C34</f>
-        <v>-48107243</v>
+        <v>0</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>7</v>
@@ -1254,10 +1258,12 @@
       <c r="B37" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1">
+        <v>4233902</v>
+      </c>
       <c r="D37" s="2">
         <f>C37-C35</f>
-        <v>-4233902</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>

</xml_diff>